<commit_message>
ip adress assignment works
</commit_message>
<xml_diff>
--- a/doc/IPRouter.xlsx
+++ b/doc/IPRouter.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="38115" windowHeight="17445"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="38115" windowHeight="17445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="ToDo" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>W5500</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>+3.3V</t>
+  </si>
+  <si>
+    <t>PID_MSG_TRANSMIT_TO_KNX</t>
+  </si>
+  <si>
+    <t>PID_MSG_TRANSMIT_TO_IP</t>
+  </si>
+  <si>
+    <t>check 03_08_03</t>
   </si>
 </sst>
 </file>
@@ -549,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
@@ -685,12 +694,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C5:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>